<commit_message>
Add groups and promotion
</commit_message>
<xml_diff>
--- a/examparams.xlsx
+++ b/examparams.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Remacle.Max\Documents\ERM\1Ma\DS425\project\ExamTimetable\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Romain\Documents\ERM\1Ma\DS425_E\Practicals_work\Projects\ExamTimetable\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3191DD58-83A6-4FBD-89F9-67313B87C452}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F5D1B60-0FE7-45C7-8FBD-FE230B6A9B1C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{6AAF5D83-5F9A-451D-AF9D-F669C897DA23}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
     <sheet name="Feuil2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="27">
   <si>
     <t>Name</t>
   </si>
@@ -95,6 +95,18 @@
   </si>
   <si>
     <t>no</t>
+  </si>
+  <si>
+    <t>Promotions</t>
+  </si>
+  <si>
+    <t>Groups</t>
+  </si>
+  <si>
+    <t>BHK=pilot</t>
+  </si>
+  <si>
+    <t>BHK=navy</t>
   </si>
 </sst>
 </file>
@@ -155,14 +167,16 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{20A04D88-210D-4F76-9832-3D7C7F78A672}" name="Tableau1" displayName="Tableau1" ref="A1:H7" totalsRowShown="0">
-  <autoFilter ref="A1:H7" xr:uid="{271BE314-FB4C-4F83-A88F-2378D6CD0FE6}"/>
-  <tableColumns count="8">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{20A04D88-210D-4F76-9832-3D7C7F78A672}" name="Tableau1" displayName="Tableau1" ref="A1:J7" totalsRowShown="0">
+  <autoFilter ref="A1:J7" xr:uid="{271BE314-FB4C-4F83-A88F-2378D6CD0FE6}"/>
+  <tableColumns count="10">
     <tableColumn id="1" xr3:uid="{4367A2A3-B526-4DFE-BBC0-E782C81177FE}" name="Name"/>
     <tableColumn id="2" xr3:uid="{905D431B-0F73-4320-B39E-29B4879E1E48}" name="Unavailability"/>
     <tableColumn id="3" xr3:uid="{B220EB76-B6B6-4904-9913-D70A0987ACC0}" name="Amount days"/>
     <tableColumn id="4" xr3:uid="{114D82F1-6DDA-417B-B75E-E81CD5F3914E}" name="preparation days"/>
     <tableColumn id="5" xr3:uid="{C78B1ED7-71E3-42F8-B8B2-26D15C6C67E1}" name="oral/written"/>
+    <tableColumn id="9" xr3:uid="{722D798A-9990-433B-A7B4-97C9CCB42EE8}" name="Promotions"/>
+    <tableColumn id="10" xr3:uid="{F37C444E-0C69-4ADB-BE4C-545730041000}" name="Groups"/>
     <tableColumn id="6" xr3:uid="{72DED2BE-4ABF-4220-A9E6-515EA9546078}" name="start date"/>
     <tableColumn id="7" xr3:uid="{C10AF50F-4281-4999-BEDB-DB655313C33E}" name="final date"/>
     <tableColumn id="8" xr3:uid="{59FE2777-4DBF-4D6E-8670-51DFDC352952}" name="is weekend ok?"/>
@@ -468,10 +482,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C068238-1761-435B-986C-4B74602C0523}">
-  <dimension ref="A1:I7"/>
+  <dimension ref="A1:K7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -479,11 +493,12 @@
     <col min="2" max="2" width="22.21875" customWidth="1"/>
     <col min="3" max="3" width="18.33203125" customWidth="1"/>
     <col min="4" max="4" width="22.33203125" customWidth="1"/>
-    <col min="5" max="5" width="15.33203125" customWidth="1"/>
-    <col min="8" max="8" width="23.33203125" customWidth="1"/>
+    <col min="5" max="7" width="15.33203125" customWidth="1"/>
+    <col min="8" max="8" width="11.21875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="23.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -500,16 +515,22 @@
         <v>9</v>
       </c>
       <c r="F1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G1" t="s">
+        <v>24</v>
+      </c>
+      <c r="H1" t="s">
         <v>12</v>
       </c>
-      <c r="G1" t="s">
+      <c r="I1" t="s">
         <v>13</v>
       </c>
-      <c r="H1" t="s">
+      <c r="J1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -525,20 +546,26 @@
       <c r="E2" t="s">
         <v>10</v>
       </c>
-      <c r="F2" s="3">
+      <c r="F2">
+        <v>172</v>
+      </c>
+      <c r="G2" t="s">
+        <v>25</v>
+      </c>
+      <c r="H2" s="3">
         <v>44346</v>
       </c>
-      <c r="G2" s="3">
+      <c r="I2" s="3">
         <v>44367</v>
       </c>
-      <c r="H2" t="s">
+      <c r="J2" t="s">
         <v>21</v>
       </c>
-      <c r="I2" t="s">
+      <c r="K2" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -554,14 +581,17 @@
       <c r="E3" t="s">
         <v>10</v>
       </c>
-      <c r="H3" t="s">
+      <c r="F3">
+        <v>172</v>
+      </c>
+      <c r="J3" t="s">
         <v>21</v>
       </c>
-      <c r="I3" t="s">
+      <c r="K3" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -577,14 +607,20 @@
       <c r="E4" t="s">
         <v>10</v>
       </c>
-      <c r="H4" t="s">
+      <c r="F4">
+        <v>172</v>
+      </c>
+      <c r="G4" t="s">
+        <v>26</v>
+      </c>
+      <c r="J4" t="s">
         <v>21</v>
       </c>
-      <c r="I4" s="2" t="s">
+      <c r="K4" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -600,14 +636,17 @@
       <c r="E5" t="s">
         <v>11</v>
       </c>
-      <c r="H5" t="s">
+      <c r="F5">
+        <v>172</v>
+      </c>
+      <c r="J5" t="s">
         <v>21</v>
       </c>
-      <c r="I5" s="2" t="s">
+      <c r="K5" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -623,11 +662,14 @@
       <c r="E6" t="s">
         <v>10</v>
       </c>
-      <c r="H6" t="s">
+      <c r="F6">
+        <v>172</v>
+      </c>
+      <c r="J6" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -643,17 +685,20 @@
       <c r="E7" t="s">
         <v>11</v>
       </c>
-      <c r="H7" t="s">
+      <c r="F7">
+        <v>172</v>
+      </c>
+      <c r="J7" t="s">
         <v>21</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E7" xr:uid="{DAF3A89F-B13B-4156-9188-B9D9D7164842}">
-      <formula1>$I$4:$I$5</formula1>
+      <formula1>$K$4:$K$5</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H2:H7" xr:uid="{F0015C6C-071C-44EB-B78C-BF7A2D05BAE2}">
-      <formula1>$I$2:$I$3</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J2:J7" xr:uid="{F0015C6C-071C-44EB-B78C-BF7A2D05BAE2}">
+      <formula1>$K$2:$K$3</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Remaster apply_prep! to use the any new constraints
</commit_message>
<xml_diff>
--- a/examparams.xlsx
+++ b/examparams.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Romain\Documents\ERM\1Ma\DS425_E\Practicals_work\Projects\ExamTimetable\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F5D1B60-0FE7-45C7-8FBD-FE230B6A9B1C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{765F8940-DB29-4F04-9A10-8639412C2604}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{6AAF5D83-5F9A-451D-AF9D-F669C897DA23}"/>
   </bookViews>
@@ -485,7 +485,7 @@
   <dimension ref="A1:K7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
patch import excel with weekend
</commit_message>
<xml_diff>
--- a/examparams.xlsx
+++ b/examparams.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Romain\Documents\ERM\1Ma\DS425_E\Practicals_work\Projects\ExamTimetable\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{765F8940-DB29-4F04-9A10-8639412C2604}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2177FEB7-AEEF-4532-8442-36B0F4F91C12}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{6AAF5D83-5F9A-451D-AF9D-F669C897DA23}"/>
   </bookViews>
@@ -485,7 +485,7 @@
   <dimension ref="A1:K7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Exams close to each other part1
</commit_message>
<xml_diff>
--- a/examparams.xlsx
+++ b/examparams.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Romain\Documents\ERM\1Ma\DS425_E\Practicals_work\Projects\ExamTimetable\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2177FEB7-AEEF-4532-8442-36B0F4F91C12}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C684EF06-A48A-4323-8618-F2BB12EFE521}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{6AAF5D83-5F9A-451D-AF9D-F669C897DA23}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="28">
   <si>
     <t>Name</t>
   </si>
@@ -107,6 +107,9 @@
   </si>
   <si>
     <t>BHK=navy</t>
+  </si>
+  <si>
+    <t>Close to</t>
   </si>
 </sst>
 </file>
@@ -167,9 +170,9 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{20A04D88-210D-4F76-9832-3D7C7F78A672}" name="Tableau1" displayName="Tableau1" ref="A1:J7" totalsRowShown="0">
-  <autoFilter ref="A1:J7" xr:uid="{271BE314-FB4C-4F83-A88F-2378D6CD0FE6}"/>
-  <tableColumns count="10">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{20A04D88-210D-4F76-9832-3D7C7F78A672}" name="Tableau1" displayName="Tableau1" ref="A1:K7" totalsRowShown="0">
+  <autoFilter ref="A1:K7" xr:uid="{271BE314-FB4C-4F83-A88F-2378D6CD0FE6}"/>
+  <tableColumns count="11">
     <tableColumn id="1" xr3:uid="{4367A2A3-B526-4DFE-BBC0-E782C81177FE}" name="Name"/>
     <tableColumn id="2" xr3:uid="{905D431B-0F73-4320-B39E-29B4879E1E48}" name="Unavailability"/>
     <tableColumn id="3" xr3:uid="{B220EB76-B6B6-4904-9913-D70A0987ACC0}" name="Amount days"/>
@@ -179,6 +182,7 @@
     <tableColumn id="10" xr3:uid="{F37C444E-0C69-4ADB-BE4C-545730041000}" name="Groups"/>
     <tableColumn id="6" xr3:uid="{72DED2BE-4ABF-4220-A9E6-515EA9546078}" name="start date"/>
     <tableColumn id="7" xr3:uid="{C10AF50F-4281-4999-BEDB-DB655313C33E}" name="final date"/>
+    <tableColumn id="12" xr3:uid="{0984FC58-BD90-4877-9089-A4CD196595DD}" name="Close to"/>
     <tableColumn id="8" xr3:uid="{59FE2777-4DBF-4D6E-8670-51DFDC352952}" name="is weekend ok?"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -482,10 +486,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C068238-1761-435B-986C-4B74602C0523}">
-  <dimension ref="A1:K7"/>
+  <dimension ref="A1:L7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+      <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -495,10 +499,10 @@
     <col min="4" max="4" width="22.33203125" customWidth="1"/>
     <col min="5" max="7" width="15.33203125" customWidth="1"/>
     <col min="8" max="8" width="11.21875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="23.33203125" customWidth="1"/>
+    <col min="11" max="11" width="23.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -527,10 +531,13 @@
         <v>13</v>
       </c>
       <c r="J1" t="s">
+        <v>27</v>
+      </c>
+      <c r="K1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -558,14 +565,17 @@
       <c r="I2" s="3">
         <v>44367</v>
       </c>
-      <c r="J2" t="s">
-        <v>21</v>
+      <c r="J2" s="3" t="s">
+        <v>6</v>
       </c>
       <c r="K2" t="s">
         <v>21</v>
       </c>
+      <c r="L2" t="s">
+        <v>21</v>
+      </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -584,14 +594,14 @@
       <c r="F3">
         <v>172</v>
       </c>
-      <c r="J3" t="s">
+      <c r="K3" t="s">
         <v>21</v>
       </c>
-      <c r="K3" t="s">
+      <c r="L3" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -613,14 +623,14 @@
       <c r="G4" t="s">
         <v>26</v>
       </c>
-      <c r="J4" t="s">
+      <c r="K4" t="s">
         <v>21</v>
       </c>
-      <c r="K4" s="2" t="s">
+      <c r="L4" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -639,14 +649,14 @@
       <c r="F5">
         <v>172</v>
       </c>
-      <c r="J5" t="s">
+      <c r="K5" t="s">
         <v>21</v>
       </c>
-      <c r="K5" s="2" t="s">
+      <c r="L5" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -665,11 +675,11 @@
       <c r="F6">
         <v>172</v>
       </c>
-      <c r="J6" t="s">
+      <c r="K6" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -688,17 +698,17 @@
       <c r="F7">
         <v>172</v>
       </c>
-      <c r="J7" t="s">
+      <c r="K7" t="s">
         <v>21</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E7" xr:uid="{DAF3A89F-B13B-4156-9188-B9D9D7164842}">
-      <formula1>$K$4:$K$5</formula1>
+      <formula1>$L$4:$L$5</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J2:J7" xr:uid="{F0015C6C-071C-44EB-B78C-BF7A2D05BAE2}">
-      <formula1>$K$2:$K$3</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K2:K7" xr:uid="{F0015C6C-071C-44EB-B78C-BF7A2D05BAE2}">
+      <formula1>$L$2:$L$3</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Oral/written and its interactions with groups
</commit_message>
<xml_diff>
--- a/examparams.xlsx
+++ b/examparams.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Romain\Documents\ERM\1Ma\DS425_E\Practicals_work\Projects\ExamTimetable\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C684EF06-A48A-4323-8618-F2BB12EFE521}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1175A4A1-9C8C-4872-9B5D-2BC3E52655D0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{6AAF5D83-5F9A-451D-AF9D-F669C897DA23}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="31">
   <si>
     <t>Name</t>
   </si>
@@ -100,16 +100,25 @@
     <t>Promotions</t>
   </si>
   <si>
-    <t>Groups</t>
-  </si>
-  <si>
     <t>BHK=pilot</t>
   </si>
   <si>
     <t>BHK=navy</t>
   </si>
   <si>
-    <t>Close to</t>
+    <t>Student groups</t>
+  </si>
+  <si>
+    <t>Course group</t>
+  </si>
+  <si>
+    <t>SE422_written</t>
+  </si>
+  <si>
+    <t>SE422_oral_1</t>
+  </si>
+  <si>
+    <t>SE422_oral_2</t>
   </si>
 </sst>
 </file>
@@ -170,8 +179,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{20A04D88-210D-4F76-9832-3D7C7F78A672}" name="Tableau1" displayName="Tableau1" ref="A1:K7" totalsRowShown="0">
-  <autoFilter ref="A1:K7" xr:uid="{271BE314-FB4C-4F83-A88F-2378D6CD0FE6}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{20A04D88-210D-4F76-9832-3D7C7F78A672}" name="Tableau1" displayName="Tableau1" ref="A1:K9" totalsRowShown="0">
+  <autoFilter ref="A1:K9" xr:uid="{271BE314-FB4C-4F83-A88F-2378D6CD0FE6}"/>
   <tableColumns count="11">
     <tableColumn id="1" xr3:uid="{4367A2A3-B526-4DFE-BBC0-E782C81177FE}" name="Name"/>
     <tableColumn id="2" xr3:uid="{905D431B-0F73-4320-B39E-29B4879E1E48}" name="Unavailability"/>
@@ -179,10 +188,10 @@
     <tableColumn id="4" xr3:uid="{114D82F1-6DDA-417B-B75E-E81CD5F3914E}" name="preparation days"/>
     <tableColumn id="5" xr3:uid="{C78B1ED7-71E3-42F8-B8B2-26D15C6C67E1}" name="oral/written"/>
     <tableColumn id="9" xr3:uid="{722D798A-9990-433B-A7B4-97C9CCB42EE8}" name="Promotions"/>
-    <tableColumn id="10" xr3:uid="{F37C444E-0C69-4ADB-BE4C-545730041000}" name="Groups"/>
+    <tableColumn id="10" xr3:uid="{F37C444E-0C69-4ADB-BE4C-545730041000}" name="Student groups"/>
     <tableColumn id="6" xr3:uid="{72DED2BE-4ABF-4220-A9E6-515EA9546078}" name="start date"/>
     <tableColumn id="7" xr3:uid="{C10AF50F-4281-4999-BEDB-DB655313C33E}" name="final date"/>
-    <tableColumn id="12" xr3:uid="{0984FC58-BD90-4877-9089-A4CD196595DD}" name="Close to"/>
+    <tableColumn id="12" xr3:uid="{0984FC58-BD90-4877-9089-A4CD196595DD}" name="Course group"/>
     <tableColumn id="8" xr3:uid="{59FE2777-4DBF-4D6E-8670-51DFDC352952}" name="is weekend ok?"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -486,19 +495,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C068238-1761-435B-986C-4B74602C0523}">
-  <dimension ref="A1:L7"/>
+  <dimension ref="A1:L9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J3" sqref="J3"/>
+      <selection activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
+    <col min="1" max="1" width="15.77734375" customWidth="1"/>
     <col min="2" max="2" width="22.21875" customWidth="1"/>
     <col min="3" max="3" width="18.33203125" customWidth="1"/>
     <col min="4" max="4" width="22.33203125" customWidth="1"/>
-    <col min="5" max="7" width="15.33203125" customWidth="1"/>
+    <col min="5" max="6" width="15.33203125" customWidth="1"/>
+    <col min="7" max="7" width="17.88671875" customWidth="1"/>
     <col min="8" max="8" width="11.21875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.33203125" customWidth="1"/>
     <col min="11" max="11" width="23.33203125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -522,7 +534,7 @@
         <v>23</v>
       </c>
       <c r="G1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="H1" t="s">
         <v>12</v>
@@ -557,7 +569,7 @@
         <v>172</v>
       </c>
       <c r="G2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H2" s="3">
         <v>44346</v>
@@ -565,9 +577,7 @@
       <c r="I2" s="3">
         <v>44367</v>
       </c>
-      <c r="J2" s="3" t="s">
-        <v>6</v>
-      </c>
+      <c r="J2" s="3"/>
       <c r="K2" t="s">
         <v>21</v>
       </c>
@@ -577,13 +587,13 @@
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>4</v>
+        <v>29</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>18</v>
       </c>
       <c r="C3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D3">
         <v>3</v>
@@ -594,6 +604,9 @@
       <c r="F3">
         <v>172</v>
       </c>
+      <c r="J3" t="s">
+        <v>4</v>
+      </c>
       <c r="K3" t="s">
         <v>21</v>
       </c>
@@ -603,16 +616,16 @@
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" t="s">
-        <v>14</v>
+        <v>30</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>18</v>
       </c>
       <c r="C4">
         <v>2</v>
       </c>
       <c r="D4">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E4" t="s">
         <v>10</v>
@@ -620,8 +633,8 @@
       <c r="F4">
         <v>172</v>
       </c>
-      <c r="G4" t="s">
-        <v>26</v>
+      <c r="J4" t="s">
+        <v>4</v>
       </c>
       <c r="K4" t="s">
         <v>21</v>
@@ -632,23 +645,26 @@
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D5">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F5">
         <v>172</v>
       </c>
+      <c r="G5" t="s">
+        <v>25</v>
+      </c>
       <c r="K5" t="s">
         <v>21</v>
       </c>
@@ -658,19 +674,19 @@
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B6" t="s">
         <v>15</v>
       </c>
       <c r="C6">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D6">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E6" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F6">
         <v>172</v>
@@ -681,19 +697,19 @@
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B7" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C7">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D7">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F7">
         <v>172</v>
@@ -702,12 +718,61 @@
         <v>21</v>
       </c>
     </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" t="s">
+        <v>19</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="D8">
+        <v>2</v>
+      </c>
+      <c r="E8" t="s">
+        <v>11</v>
+      </c>
+      <c r="F8">
+        <v>172</v>
+      </c>
+      <c r="K8" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>28</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9">
+        <v>1</v>
+      </c>
+      <c r="D9">
+        <v>3</v>
+      </c>
+      <c r="E9" t="s">
+        <v>11</v>
+      </c>
+      <c r="F9">
+        <v>172</v>
+      </c>
+      <c r="J9" t="s">
+        <v>4</v>
+      </c>
+      <c r="K9" t="s">
+        <v>21</v>
+      </c>
+    </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E7" xr:uid="{DAF3A89F-B13B-4156-9188-B9D9D7164842}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E9" xr:uid="{DAF3A89F-B13B-4156-9188-B9D9D7164842}">
       <formula1>$L$4:$L$5</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K2:K7" xr:uid="{F0015C6C-071C-44EB-B78C-BF7A2D05BAE2}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K2:K9" xr:uid="{F0015C6C-071C-44EB-B78C-BF7A2D05BAE2}">
       <formula1>$L$2:$L$3</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Changes in examparams to make solution possible
</commit_message>
<xml_diff>
--- a/examparams.xlsx
+++ b/examparams.xlsx
@@ -15,17 +15,17 @@
   <calcPr/>
   <extLst>
     <ext uri="smNativeData">
-      <pm:revision xmlns:pm="smNativeData" day="1617823326" val="982" rev="124" rev64="64" revOS="3" revMin="124" revMax="0"/>
-      <pm:docPrefs xmlns:pm="smNativeData" id="1617823326" fixedDigits="0" showNotice="1" showFrameBounds="1" autoChart="1" recalcOnPrint="1" recalcOnCopy="1" finalRounding="1" compatTextArt="1" tab="567" useDefinedPrintRange="1" printArea="currentSheet"/>
-      <pm:compatibility xmlns:pm="smNativeData" id="1617823326" overlapCells="1"/>
-      <pm:defCurrency xmlns:pm="smNativeData" id="1617823326"/>
+      <pm:revision xmlns:pm="smNativeData" day="1617825070" val="982" rev="124" rev64="64" revOS="3" revMin="124" revMax="0"/>
+      <pm:docPrefs xmlns:pm="smNativeData" id="1617825070" fixedDigits="0" showNotice="1" showFrameBounds="1" autoChart="1" recalcOnPrint="1" recalcOnCopy="1" finalRounding="1" compatTextArt="1" tab="567" useDefinedPrintRange="1" printArea="currentSheet"/>
+      <pm:compatibility xmlns:pm="smNativeData" id="1617825070" overlapCells="1"/>
+      <pm:defCurrency xmlns:pm="smNativeData" id="1617825070"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="54">
   <si>
     <t>Semaine</t>
   </si>
@@ -102,94 +102,88 @@
     <t>WA421</t>
   </si>
   <si>
+    <t>oral</t>
+  </si>
+  <si>
+    <t>BHK=pilot</t>
+  </si>
+  <si>
+    <t>no</t>
+  </si>
+  <si>
+    <t>SE422_oral_1</t>
+  </si>
+  <si>
+    <t>SE422</t>
+  </si>
+  <si>
+    <t>SE422_oral_2</t>
+  </si>
+  <si>
+    <t>TN423</t>
+  </si>
+  <si>
+    <t>BHK=navy</t>
+  </si>
+  <si>
+    <t>TP424</t>
+  </si>
+  <si>
+    <t>written</t>
+  </si>
+  <si>
+    <t>DS425</t>
+  </si>
+  <si>
+    <t>30-&gt;5</t>
+  </si>
+  <si>
+    <t>SE426</t>
+  </si>
+  <si>
+    <t>SE422_written</t>
+  </si>
+  <si>
+    <t>yes</t>
+  </si>
+  <si>
+    <t>cours de smeuh 1</t>
+  </si>
+  <si>
     <t>13; 14;15</t>
   </si>
   <si>
-    <t>oral</t>
-  </si>
-  <si>
-    <t>BHK=pilot</t>
-  </si>
-  <si>
-    <t>no</t>
-  </si>
-  <si>
-    <t>SE422_oral_1</t>
-  </si>
-  <si>
-    <t>30-&gt;2</t>
-  </si>
-  <si>
-    <t>SE422</t>
-  </si>
-  <si>
-    <t>SE422_oral_2</t>
-  </si>
-  <si>
-    <t>TN423</t>
-  </si>
-  <si>
-    <t>18;19</t>
-  </si>
-  <si>
-    <t>BHK=navy</t>
-  </si>
-  <si>
-    <t>TP424</t>
-  </si>
-  <si>
-    <t>16-&gt;20</t>
-  </si>
-  <si>
-    <t>written</t>
-  </si>
-  <si>
-    <t>DS425</t>
+    <t>BHK=N</t>
+  </si>
+  <si>
+    <t>cours de smeuh 2</t>
+  </si>
+  <si>
+    <t>30-&gt;2;   11 -&gt; 15</t>
+  </si>
+  <si>
+    <t>BHK=F</t>
+  </si>
+  <si>
+    <t>Teuf 1</t>
+  </si>
+  <si>
+    <t>1-&gt;10;18;19</t>
+  </si>
+  <si>
+    <t>Teuf 2</t>
   </si>
   <si>
     <t>19;20</t>
   </si>
   <si>
-    <t>SE426</t>
+    <t>Teuf 3</t>
+  </si>
+  <si>
+    <t>gueule de bois</t>
   </si>
   <si>
     <t>17-&gt;20</t>
-  </si>
-  <si>
-    <t>SE422_written</t>
-  </si>
-  <si>
-    <t>30-&gt;2;   11 -&gt; 15</t>
-  </si>
-  <si>
-    <t>yes</t>
-  </si>
-  <si>
-    <t>cours de smeuh 1</t>
-  </si>
-  <si>
-    <t>BHK=N</t>
-  </si>
-  <si>
-    <t>cours de smeuh 2</t>
-  </si>
-  <si>
-    <t>BHK=F</t>
-  </si>
-  <si>
-    <t>Teuf 1</t>
-  </si>
-  <si>
-    <t>1-&gt;10;18;19</t>
-  </si>
-  <si>
-    <t>Teuf 2</t>
-  </si>
-  <si>
-    <t>Teuf 3</t>
-  </si>
-  <si>
-    <t>gueule de bois</t>
   </si>
   <si>
     <t>Soirée Coaster</t>
@@ -220,7 +214,7 @@
       <sz val="11"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1617823326" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1617825070" ulstyle="none" kern="1">
             <pm:latin face="Calibri" sz="220" lang="default"/>
             <pm:cs face="Basic Roman" sz="220" lang="default"/>
             <pm:ea face="Basic Roman" sz="220" lang="default"/>
@@ -235,7 +229,7 @@
       <sz val="10"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1617823326" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1617825070" ulstyle="none" kern="1">
             <pm:latin face="Basic Sans" sz="200" lang="default"/>
             <pm:cs face="Basic Roman" sz="200" lang="default"/>
             <pm:ea face="Basic Roman" sz="200" lang="default"/>
@@ -251,7 +245,7 @@
       <sz val="14"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1617823326" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1617825070" ulstyle="none" kern="1">
             <pm:latin face="Calibri" sz="280" lang="default" weight="bold"/>
             <pm:cs face="Basic Roman" sz="280" lang="default" weight="bold"/>
             <pm:ea face="Basic Roman" sz="280" lang="default" weight="bold"/>
@@ -294,7 +288,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1617823326" type="1" fgLvl="100" fgClr="00000000" bgLvl="100" bgClr="00000000"/>
+            <pm:shade xmlns:pm="smNativeData" id="1617825070" type="1" fgLvl="100" fgClr="00000000" bgLvl="100" bgClr="00000000"/>
           </ext>
         </extLst>
       </patternFill>
@@ -305,7 +299,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1617823326" type="1" fgLvl="100" fgClr="00FFFFFF" bgLvl="100" bgClr="00000000"/>
+            <pm:shade xmlns:pm="smNativeData" id="1617825070" type="1" fgLvl="100" fgClr="00FFFFFF" bgLvl="100" bgClr="00000000"/>
           </ext>
         </extLst>
       </patternFill>
@@ -327,7 +321,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1617823326"/>
+          <pm:border xmlns:pm="smNativeData" id="1617825070"/>
         </ext>
       </extLst>
     </border>
@@ -346,7 +340,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1617823326">
+          <pm:border xmlns:pm="smNativeData" id="1617825070">
             <pm:line position="top" type="1" style="0" width="30" dist="20" width2="20" rgb="000000"/>
             <pm:line position="left" type="1" style="0" width="30" dist="20" width2="20" rgb="000000"/>
             <pm:line position="right" type="1" style="0" width="30" dist="20" width2="20" rgb="000000"/>
@@ -369,7 +363,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1617823326">
+          <pm:border xmlns:pm="smNativeData" id="1617825070">
             <pm:line position="bottom" type="1" style="0" width="30" dist="20" width2="20" rgb="000000"/>
             <pm:line position="left" type="1" style="0" width="30" dist="20" width2="20" rgb="000000"/>
             <pm:line position="right" type="1" style="0" width="30" dist="20" width2="20" rgb="000000"/>
@@ -392,7 +386,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1617823326">
+          <pm:border xmlns:pm="smNativeData" id="1617825070">
             <pm:line position="top" type="1" style="0" width="30" dist="20" width2="20" rgb="000000"/>
             <pm:line position="bottom" type="1" style="0" width="30" dist="20" width2="20" rgb="000000"/>
             <pm:line position="left" type="1" style="0" width="30" dist="20" width2="20" rgb="000000"/>
@@ -415,7 +409,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1617823326">
+          <pm:border xmlns:pm="smNativeData" id="1617825070">
             <pm:line position="top" type="1" style="0" width="30" dist="20" width2="20" rgb="000000"/>
             <pm:line position="bottom" type="1" style="0" width="30" dist="20" width2="20" rgb="000000"/>
           </pm:border>
@@ -437,7 +431,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1617823326">
+          <pm:border xmlns:pm="smNativeData" id="1617825070">
             <pm:line position="top" type="1" style="0" width="30" dist="20" width2="20" rgb="000000"/>
             <pm:line position="bottom" type="1" style="0" width="30" dist="20" width2="20" rgb="000000"/>
             <pm:line position="right" type="1" style="0" width="30" dist="20" width2="20" rgb="000000"/>
@@ -460,7 +454,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1617823326">
+          <pm:border xmlns:pm="smNativeData" id="1617825070">
             <pm:line position="top" type="1" style="0" width="30" dist="20" width2="20" rgb="000000"/>
             <pm:line position="bottom" type="1" style="0" width="30" dist="20" width2="20" rgb="000000"/>
             <pm:line position="left" type="1" style="0" width="30" dist="20" width2="20" rgb="000000"/>
@@ -484,7 +478,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1617823326">
+          <pm:border xmlns:pm="smNativeData" id="1617825070">
             <pm:line position="right" type="1" style="0" width="30" dist="20" width2="20" rgb="000000"/>
           </pm:border>
         </ext>
@@ -505,7 +499,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1617823326"/>
+          <pm:border xmlns:pm="smNativeData" id="1617825070"/>
         </ext>
       </extLst>
     </border>
@@ -524,7 +518,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1617823326"/>
+          <pm:border xmlns:pm="smNativeData" id="1617825070"/>
         </ext>
       </extLst>
     </border>
@@ -563,7 +557,7 @@
           <bgColor rgb="FFE26B0A"/>
           <extLst>
             <ext uri="smNativeData">
-              <pm:shade xmlns:pm="smNativeData" id="1617823326" type="1" fgLvl="100" fgClr="00E26B0A" bgLvl="100" bgClr="FFFFFFFF"/>
+              <pm:shade xmlns:pm="smNativeData" id="1617825070" type="1" fgLvl="100" fgClr="00E26B0A" bgLvl="100" bgClr="FFFFFFFF"/>
             </ext>
           </extLst>
         </patternFill>
@@ -575,7 +569,7 @@
           <bgColor rgb="FFC2D69A"/>
           <extLst>
             <ext uri="smNativeData">
-              <pm:shade xmlns:pm="smNativeData" id="1617823326" type="1" fgLvl="100" fgClr="00C2D69A" bgLvl="100" bgClr="FFFFFFFF"/>
+              <pm:shade xmlns:pm="smNativeData" id="1617825070" type="1" fgLvl="100" fgClr="00C2D69A" bgLvl="100" bgClr="FFFFFFFF"/>
             </ext>
           </extLst>
         </patternFill>
@@ -585,10 +579,10 @@
   <tableStyles count="0"/>
   <extLst>
     <ext uri="smNativeData">
-      <pm:charStyles xmlns:pm="smNativeData" id="1617823326" count="1">
+      <pm:charStyles xmlns:pm="smNativeData" id="1617825070" count="1">
         <pm:charStyle name="Normal" fontId="0" Id="1"/>
       </pm:charStyles>
-      <pm:colors xmlns:pm="smNativeData" id="1617823326" count="2">
+      <pm:colors xmlns:pm="smNativeData" id="1617825070" count="2">
         <pm:color name="Color 24" rgb="E26B0A"/>
         <pm:color name="Color 25" rgb="C2D69A"/>
       </pm:colors>
@@ -906,7 +900,7 @@
     <col min="3" max="3" width="6.553571" hidden="1" customWidth="1">
       <extLst>
         <ext uri="smNativeData">
-          <pm:columnDef xmlns:pm="smNativeData" id="1617823326" min="3" max="3" hidden="1" collapsedDB="0" collapsedOL="0"/>
+          <pm:columnDef xmlns:pm="smNativeData" id="1617825070" min="3" max="3" hidden="1" collapsedDB="0" collapsedOL="0"/>
         </ext>
       </extLst>
     </col>
@@ -1697,7 +1691,7 @@
   <printOptions>
     <extLst>
       <ext uri="smNativeData">
-        <pm:pageFlags xmlns:pm="smNativeData" id="1617823326" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
+        <pm:pageFlags xmlns:pm="smNativeData" id="1617825070" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
       </ext>
     </extLst>
   </printOptions>
@@ -1706,14 +1700,14 @@
   <headerFooter>
     <extLst>
       <ext uri="smNativeData">
-        <pm:header xmlns:pm="smNativeData" id="1617823326" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
-        <pm:footer xmlns:pm="smNativeData" id="1617823326" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
+        <pm:header xmlns:pm="smNativeData" id="1617825070" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
+        <pm:footer xmlns:pm="smNativeData" id="1617825070" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
       </ext>
     </extLst>
   </headerFooter>
   <extLst>
     <ext uri="smNativeData">
-      <pm:sheetPrefs xmlns:pm="smNativeData" day="1617823326" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
+      <pm:sheetPrefs xmlns:pm="smNativeData" day="1617825070" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
         <pm:shade id="0" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
         <pm:shade id="1" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
       </pm:sheetPrefs>
@@ -1727,14 +1721,14 @@
   <dimension ref="A1:K38"/>
   <sheetViews>
     <sheetView tabSelected="1" view="normal" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.660714" defaultRowHeight="15.40"/>
   <cols>
     <col min="1" max="1" width="15.776786" customWidth="1"/>
     <col min="2" max="2" width="16.437500" customWidth="1"/>
-    <col min="3" max="3" width="5.883929" customWidth="1"/>
+    <col min="3" max="3" width="18.107143" customWidth="1"/>
     <col min="4" max="4" width="22.330357" customWidth="1"/>
     <col min="5" max="6" width="15.330357" customWidth="1"/>
     <col min="7" max="7" width="17.883929" customWidth="1"/>
@@ -1782,9 +1776,7 @@
       <c r="A2" t="s">
         <v>24</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>25</v>
-      </c>
+      <c r="B2" s="1"/>
       <c r="C2" t="n">
         <v>1</v>
       </c>
@@ -1792,13 +1784,13 @@
         <v>1</v>
       </c>
       <c r="E2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F2" t="n">
         <v>172</v>
       </c>
       <c r="G2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H2" s="3" t="n">
         <v>44346</v>
@@ -1808,94 +1800,86 @@
       </c>
       <c r="J2" s="3"/>
       <c r="K2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="3" spans="1:11">
       <c r="A3" t="s">
-        <v>29</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>30</v>
-      </c>
+        <v>28</v>
+      </c>
+      <c r="B3" s="1"/>
       <c r="C3" t="n">
         <v>2</v>
       </c>
       <c r="D3" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F3" t="n">
         <v>172</v>
       </c>
       <c r="J3" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="K3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="4" spans="1:11">
       <c r="A4" t="s">
-        <v>32</v>
-      </c>
-      <c r="B4" s="1" t="s">
         <v>30</v>
       </c>
+      <c r="B4" s="1"/>
       <c r="C4" t="n">
         <v>2</v>
       </c>
       <c r="D4" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F4" t="n">
         <v>172</v>
       </c>
       <c r="J4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="K4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="5" spans="1:11">
       <c r="A5" t="s">
-        <v>33</v>
-      </c>
-      <c r="B5" t="s">
-        <v>34</v>
-      </c>
+        <v>31</v>
+      </c>
+      <c r="B5" s="1"/>
       <c r="C5" t="n">
         <v>2</v>
       </c>
       <c r="D5" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F5" t="n">
         <v>172</v>
       </c>
       <c r="G5" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="K5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="6" spans="1:11">
       <c r="A6" t="s">
-        <v>36</v>
-      </c>
-      <c r="B6" s="12" t="s">
-        <v>37</v>
-      </c>
+        <v>33</v>
+      </c>
+      <c r="B6" s="1"/>
       <c r="C6" t="n">
         <v>1</v>
       </c>
@@ -1903,105 +1887,101 @@
         <v>1</v>
       </c>
       <c r="E6" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="F6" t="n">
         <v>172</v>
       </c>
       <c r="K6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="7" spans="1:11">
       <c r="A7" t="s">
-        <v>39</v>
-      </c>
-      <c r="B7" t="s">
-        <v>40</v>
+        <v>35</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>36</v>
       </c>
       <c r="C7" t="n">
         <v>3</v>
       </c>
       <c r="D7" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F7" t="n">
         <v>172</v>
       </c>
       <c r="K7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="8" spans="1:11">
       <c r="A8" t="s">
-        <v>41</v>
-      </c>
-      <c r="B8" t="s">
-        <v>42</v>
-      </c>
+        <v>37</v>
+      </c>
+      <c r="B8" s="1"/>
       <c r="C8" t="n">
         <v>1</v>
       </c>
       <c r="D8" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E8" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="F8" t="n">
         <v>172</v>
       </c>
       <c r="K8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="9" spans="1:11">
       <c r="A9" t="s">
-        <v>43</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>44</v>
-      </c>
+        <v>38</v>
+      </c>
+      <c r="B9" s="1"/>
       <c r="C9" t="n">
         <v>1</v>
       </c>
       <c r="D9" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E9" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="F9" t="n">
         <v>172</v>
       </c>
       <c r="J9" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="K9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="35" spans="1:1">
       <c r="A35" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
     </row>
     <row r="36" spans="1:1">
       <c r="A36" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="37" spans="1:1">
       <c r="A37" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="38" spans="1:1">
       <c r="A38" s="2" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>
@@ -2016,7 +1996,7 @@
   <printOptions>
     <extLst>
       <ext uri="smNativeData">
-        <pm:pageFlags xmlns:pm="smNativeData" id="1617823326" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
+        <pm:pageFlags xmlns:pm="smNativeData" id="1617825070" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
       </ext>
     </extLst>
   </printOptions>
@@ -2025,8 +2005,8 @@
   <headerFooter>
     <extLst>
       <ext uri="smNativeData">
-        <pm:header xmlns:pm="smNativeData" id="1617823326" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
-        <pm:footer xmlns:pm="smNativeData" id="1617823326" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
+        <pm:header xmlns:pm="smNativeData" id="1617825070" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
+        <pm:footer xmlns:pm="smNativeData" id="1617825070" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
       </ext>
     </extLst>
   </headerFooter>
@@ -2035,7 +2015,7 @@
   </tableParts>
   <extLst>
     <ext uri="smNativeData">
-      <pm:sheetPrefs xmlns:pm="smNativeData" day="1617823326" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
+      <pm:sheetPrefs xmlns:pm="smNativeData" day="1617825070" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
         <pm:shade id="0" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
         <pm:shade id="1" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
       </pm:sheetPrefs>
@@ -2099,10 +2079,10 @@
     </row>
     <row r="2" spans="1:14">
       <c r="A2" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>25</v>
+        <v>41</v>
       </c>
       <c r="C2" t="n">
         <v>1</v>
@@ -2111,13 +2091,13 @@
         <v>1</v>
       </c>
       <c r="E2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F2" t="n">
         <v>157</v>
       </c>
       <c r="G2" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="H2" s="3" t="n">
         <v>44346</v>
@@ -2127,13 +2107,13 @@
       </c>
       <c r="J2" s="3"/>
       <c r="K2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="N2" s="3"/>
     </row>
     <row r="3" spans="1:11">
       <c r="A3" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>44</v>
@@ -2145,24 +2125,24 @@
         <v>3</v>
       </c>
       <c r="E3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F3" t="n">
         <v>157</v>
       </c>
       <c r="G3" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="K3" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
     </row>
     <row r="4" spans="1:11">
       <c r="A4" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="B4" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="C4" t="n">
         <v>2</v>
@@ -2171,24 +2151,24 @@
         <v>4</v>
       </c>
       <c r="E4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F4" t="n">
         <v>157</v>
       </c>
       <c r="G4" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="K4" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
     </row>
     <row r="5" spans="1:11">
       <c r="A5" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="B5" t="s">
-        <v>40</v>
+        <v>49</v>
       </c>
       <c r="C5" t="n">
         <v>1</v>
@@ -2197,24 +2177,24 @@
         <v>1</v>
       </c>
       <c r="E5" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="F5" t="n">
         <v>157</v>
       </c>
       <c r="G5" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="K5" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
     </row>
     <row r="6" spans="1:11">
       <c r="A6" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="B6" t="s">
-        <v>40</v>
+        <v>49</v>
       </c>
       <c r="C6" t="n">
         <v>1</v>
@@ -2223,21 +2203,21 @@
         <v>4</v>
       </c>
       <c r="E6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F6" t="n">
         <v>157</v>
       </c>
       <c r="K6" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
     </row>
     <row r="7" spans="1:11">
       <c r="A7" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="B7" t="s">
-        <v>42</v>
+        <v>52</v>
       </c>
       <c r="C7" t="n">
         <v>1</v>
@@ -2246,18 +2226,18 @@
         <v>2</v>
       </c>
       <c r="E7" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="F7" t="n">
         <v>157</v>
       </c>
       <c r="K7" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
     </row>
     <row r="8" spans="1:11">
       <c r="A8" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>44</v>
@@ -2269,33 +2249,33 @@
         <v>3</v>
       </c>
       <c r="E8" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="F8" t="n">
         <v>157</v>
       </c>
       <c r="K8" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
     </row>
     <row r="29" spans="1:1">
       <c r="A29" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
     </row>
     <row r="30" spans="1:1">
       <c r="A30" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="31" spans="1:1">
       <c r="A31" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="32" spans="1:1">
       <c r="A32" s="2" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>
@@ -2310,7 +2290,7 @@
   <printOptions>
     <extLst>
       <ext uri="smNativeData">
-        <pm:pageFlags xmlns:pm="smNativeData" id="1617823326" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
+        <pm:pageFlags xmlns:pm="smNativeData" id="1617825070" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
       </ext>
     </extLst>
   </printOptions>
@@ -2319,8 +2299,8 @@
   <headerFooter>
     <extLst>
       <ext uri="smNativeData">
-        <pm:header xmlns:pm="smNativeData" id="1617823326" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
-        <pm:footer xmlns:pm="smNativeData" id="1617823326" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
+        <pm:header xmlns:pm="smNativeData" id="1617825070" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
+        <pm:footer xmlns:pm="smNativeData" id="1617825070" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
       </ext>
     </extLst>
   </headerFooter>
@@ -2329,7 +2309,7 @@
   </tableParts>
   <extLst>
     <ext uri="smNativeData">
-      <pm:sheetPrefs xmlns:pm="smNativeData" day="1617823326" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
+      <pm:sheetPrefs xmlns:pm="smNativeData" day="1617825070" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
         <pm:shade id="0" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
         <pm:shade id="1" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
       </pm:sheetPrefs>

</xml_diff>

<commit_message>
Professors added, dependency between proms coming soon
</commit_message>
<xml_diff>
--- a/examparams.xlsx
+++ b/examparams.xlsx
@@ -5,7 +5,7 @@
   <fileSharing readOnlyRecommended="0" userName="sputnik"/>
   <workbookPr/>
   <bookViews>
-    <workbookView activeTab="0" xWindow="240" yWindow="60" windowWidth="23252" windowHeight="12579" tabRatio="500"/>
+    <workbookView activeTab="1" xWindow="240" yWindow="60" windowWidth="23246" windowHeight="12578" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="172 POL" sheetId="1" r:id="rId4"/>
@@ -14,17 +14,17 @@
   <calcPr/>
   <extLst>
     <ext uri="smNativeData">
-      <pm:revision xmlns:pm="smNativeData" day="1618575011" val="982" rev="124" rev64="64" revOS="3" revMin="124" revMax="0"/>
-      <pm:docPrefs xmlns:pm="smNativeData" id="1618575011" fixedDigits="0" showNotice="1" showFrameBounds="1" autoChart="1" recalcOnPrint="1" recalcOnCopy="1" finalRounding="1" compatTextArt="1" tab="567" useDefinedPrintRange="1" printArea="currentSheet"/>
-      <pm:compatibility xmlns:pm="smNativeData" id="1618575011" overlapCells="1"/>
-      <pm:defCurrency xmlns:pm="smNativeData" id="1618575011"/>
+      <pm:revision xmlns:pm="smNativeData" day="1619371127" val="982" rev="124" rev64="64" revOS="3" revMin="124" revMax="0"/>
+      <pm:docPrefs xmlns:pm="smNativeData" id="1619371127" fixedDigits="0" showNotice="1" showFrameBounds="1" autoChart="1" recalcOnPrint="1" recalcOnCopy="1" finalRounding="1" compatTextArt="1" tab="567" useDefinedPrintRange="1" printArea="currentSheet"/>
+      <pm:compatibility xmlns:pm="smNativeData" id="1619371127" overlapCells="1"/>
+      <pm:defCurrency xmlns:pm="smNativeData" id="1619371127"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="37">
   <si>
     <t>Name</t>
   </si>
@@ -41,79 +41,76 @@
     <t>oral/written</t>
   </si>
   <si>
-    <t>Promotions</t>
+    <t>Promotion</t>
   </si>
   <si>
     <t>Student groups</t>
   </si>
   <si>
-    <t>start date</t>
-  </si>
-  <si>
-    <t>final date</t>
-  </si>
-  <si>
     <t>Course group</t>
   </si>
   <si>
-    <t>is weekend ok?</t>
-  </si>
-  <si>
     <t>WA421</t>
   </si>
   <si>
+    <t>Van Utterbeek</t>
+  </si>
+  <si>
     <t>oral</t>
   </si>
   <si>
+    <t>172POL</t>
+  </si>
+  <si>
     <t>BHK=pilot</t>
   </si>
   <si>
+    <t>SE422_oral_1</t>
+  </si>
+  <si>
+    <t>Merken</t>
+  </si>
+  <si>
+    <t>SE422</t>
+  </si>
+  <si>
+    <t>SE422_oral_2</t>
+  </si>
+  <si>
+    <t>TN423</t>
+  </si>
+  <si>
+    <t>BHK=navy</t>
+  </si>
+  <si>
+    <t>TP424</t>
+  </si>
+  <si>
+    <t>written</t>
+  </si>
+  <si>
+    <t>DS425</t>
+  </si>
+  <si>
+    <t>SE426</t>
+  </si>
+  <si>
+    <t>SE422_written</t>
+  </si>
+  <si>
+    <t>yes</t>
+  </si>
+  <si>
     <t>no</t>
   </si>
   <si>
-    <t>SE422_oral_1</t>
-  </si>
-  <si>
-    <t>Merken</t>
-  </si>
-  <si>
-    <t>SE422</t>
-  </si>
-  <si>
-    <t>SE422_oral_2</t>
-  </si>
-  <si>
-    <t>TN423</t>
-  </si>
-  <si>
-    <t>BHK=navy</t>
-  </si>
-  <si>
-    <t>TP424</t>
-  </si>
-  <si>
-    <t>written</t>
-  </si>
-  <si>
-    <t>DS425</t>
-  </si>
-  <si>
-    <t>SE426</t>
-  </si>
-  <si>
-    <t>SE422_written</t>
-  </si>
-  <si>
-    <t>yes</t>
-  </si>
-  <si>
-    <t>Unavailability</t>
-  </si>
-  <si>
     <t>cours de smeuh 1</t>
   </si>
   <si>
-    <t>13; 14;15</t>
+    <t>Pas cours</t>
+  </si>
+  <si>
+    <t>157SSMW</t>
   </si>
   <si>
     <t>BHK=N</t>
@@ -122,31 +119,19 @@
     <t>cours de smeuh 2</t>
   </si>
   <si>
-    <t>30-&gt;2;   11 -&gt; 15</t>
-  </si>
-  <si>
     <t>BHK=F</t>
   </si>
   <si>
     <t>Teuf 1</t>
   </si>
   <si>
-    <t>1-&gt;10;18;19</t>
-  </si>
-  <si>
     <t>Teuf 2</t>
   </si>
   <si>
-    <t>19;20</t>
-  </si>
-  <si>
     <t>Teuf 3</t>
   </si>
   <si>
     <t>gueule de bois</t>
-  </si>
-  <si>
-    <t>17-&gt;20</t>
   </si>
   <si>
     <t>Soirée Coaster</t>
@@ -176,7 +161,7 @@
       <sz val="11"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1618575011" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1619371127" ulstyle="none" kern="1">
             <pm:latin face="Calibri" sz="220" lang="default"/>
             <pm:cs face="Basic Roman" sz="220" lang="default"/>
             <pm:ea face="Basic Roman" sz="220" lang="default"/>
@@ -191,7 +176,7 @@
       <sz val="10"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1618575011" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1619371127" ulstyle="none" kern="1">
             <pm:latin face="Basic Sans" sz="200" lang="default"/>
             <pm:cs face="Basic Roman" sz="200" lang="default"/>
             <pm:ea face="Basic Roman" sz="200" lang="default"/>
@@ -213,7 +198,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1618575011" type="1" fgLvl="100" fgClr="00000000" bgLvl="100" bgClr="00000000"/>
+            <pm:shade xmlns:pm="smNativeData" id="1619371127" type="1" fgLvl="100" fgClr="00000000" bgLvl="100" bgClr="00000000"/>
           </ext>
         </extLst>
       </patternFill>
@@ -224,7 +209,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1618575011" type="1" fgLvl="100" fgClr="00FFFFFF" bgLvl="100" bgClr="00000000"/>
+            <pm:shade xmlns:pm="smNativeData" id="1619371127" type="1" fgLvl="100" fgClr="00FFFFFF" bgLvl="100" bgClr="00000000"/>
           </ext>
         </extLst>
       </patternFill>
@@ -246,7 +231,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1618575011"/>
+          <pm:border xmlns:pm="smNativeData" id="1619371127"/>
         </ext>
       </extLst>
     </border>
@@ -265,7 +250,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1618575011"/>
+          <pm:border xmlns:pm="smNativeData" id="1619371127"/>
         </ext>
       </extLst>
     </border>
@@ -284,7 +269,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1618575011"/>
+          <pm:border xmlns:pm="smNativeData" id="1619371127"/>
         </ext>
       </extLst>
     </border>
@@ -306,10 +291,10 @@
   <tableStyles count="0"/>
   <extLst>
     <ext uri="smNativeData">
-      <pm:charStyles xmlns:pm="smNativeData" id="1618575011" count="1">
+      <pm:charStyles xmlns:pm="smNativeData" id="1619371127" count="1">
         <pm:charStyle name="Normal" fontId="0" Id="1"/>
       </pm:charStyles>
-      <pm:colors xmlns:pm="smNativeData" id="1618575011" count="2">
+      <pm:colors xmlns:pm="smNativeData" id="1619371127" count="2">
         <pm:color name="Color 24" rgb="E26B0A"/>
         <pm:color name="Color 25" rgb="C2D69A"/>
       </pm:colors>
@@ -319,40 +304,34 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tableau1" displayName="Tableau1" ref="A1:K9" totalsRowShown="0">
-  <autoFilter ref="A1:K9"/>
-  <tableColumns count="11">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tableau1" displayName="Tableau1" ref="A1:H9" totalsRowShown="0">
+  <autoFilter ref="A1:H9"/>
+  <tableColumns count="8">
     <tableColumn id="1" name="Name" totalsRowLabel="Total"/>
     <tableColumn id="2" name="Professor"/>
     <tableColumn id="3" name="Amount days"/>
     <tableColumn id="4" name="preparation days"/>
     <tableColumn id="5" name="oral/written"/>
-    <tableColumn id="6" name="Promotions"/>
+    <tableColumn id="6" name="Promotion"/>
     <tableColumn id="7" name="Student groups"/>
-    <tableColumn id="8" name="start date"/>
-    <tableColumn id="9" name="final date"/>
-    <tableColumn id="10" name="Course group"/>
-    <tableColumn id="11" name="is weekend ok?" totalsRowFunction="sum"/>
+    <tableColumn id="8" name="Course group" totalsRowFunction="sum"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table1" displayName="Table1" ref="A1:K8" totalsRowShown="0">
-  <autoFilter ref="A1:K8"/>
-  <tableColumns count="11">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table1" displayName="Table1" ref="A1:H8" totalsRowShown="0">
+  <autoFilter ref="A1:H8"/>
+  <tableColumns count="8">
     <tableColumn id="1" name="Name" totalsRowLabel="Total"/>
-    <tableColumn id="2" name="Unavailability"/>
+    <tableColumn id="2" name="Professor"/>
     <tableColumn id="3" name="Amount days"/>
     <tableColumn id="4" name="preparation days"/>
     <tableColumn id="5" name="oral/written"/>
-    <tableColumn id="6" name="Promotions"/>
+    <tableColumn id="6" name="Promotion"/>
     <tableColumn id="7" name="Student groups"/>
-    <tableColumn id="8" name="start date"/>
-    <tableColumn id="9" name="final date"/>
-    <tableColumn id="10" name="Course group"/>
-    <tableColumn id="11" name="is weekend ok?" totalsRowFunction="sum"/>
+    <tableColumn id="8" name="Course group" totalsRowFunction="sum"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -614,10 +593,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K38"/>
+  <dimension ref="A1:I38"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="normal" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView view="normal" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3:F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.660714" defaultRowHeight="15.40"/>
@@ -628,12 +607,10 @@
     <col min="4" max="4" width="22.330357" customWidth="1"/>
     <col min="5" max="6" width="15.330357" customWidth="1"/>
     <col min="7" max="7" width="17.883929" customWidth="1"/>
-    <col min="8" max="8" width="11.214286" customWidth="1"/>
-    <col min="10" max="10" width="14.330357" customWidth="1"/>
-    <col min="11" max="11" width="23.330357" customWidth="1"/>
+    <col min="8" max="8" width="14.330357" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:9">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -658,53 +635,37 @@
       <c r="H1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+    </row>
+    <row r="2" spans="1:9">
+      <c r="A2" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="B2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
+      <c r="C2" t="n">
+        <v>1</v>
+      </c>
+      <c r="D2" t="n">
+        <v>1</v>
+      </c>
+      <c r="E2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="2" spans="1:11">
-      <c r="A2" t="s">
+      <c r="F2" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="1"/>
-      <c r="C2" t="n">
-        <v>1</v>
-      </c>
-      <c r="D2" t="n">
-        <v>1</v>
-      </c>
-      <c r="E2" t="s">
+      <c r="G2" t="s">
         <v>12</v>
       </c>
-      <c r="F2" t="n">
-        <v>172</v>
-      </c>
-      <c r="G2" t="s">
+      <c r="H2" s="3"/>
+    </row>
+    <row r="3" spans="1:9">
+      <c r="A3" t="s">
         <v>13</v>
       </c>
-      <c r="H2" s="3" t="n">
-        <v>44346</v>
-      </c>
-      <c r="I2" s="3" t="n">
-        <v>44367</v>
-      </c>
-      <c r="J2" s="3"/>
-      <c r="K2" t="s">
+      <c r="B3" s="1" t="s">
         <v>14</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11">
-      <c r="A3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>16</v>
       </c>
       <c r="C3" t="n">
         <v>2</v>
@@ -713,24 +674,21 @@
         <v>1</v>
       </c>
       <c r="E3" t="s">
-        <v>12</v>
-      </c>
-      <c r="F3" t="n">
-        <v>172</v>
-      </c>
-      <c r="J3" t="s">
-        <v>17</v>
-      </c>
-      <c r="K3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F3" t="s">
+        <v>11</v>
+      </c>
+      <c r="H3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
+      <c r="A4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>14</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11">
-      <c r="A4" t="s">
-        <v>18</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>16</v>
       </c>
       <c r="C4" t="n">
         <v>2</v>
@@ -739,23 +697,22 @@
         <v>1</v>
       </c>
       <c r="E4" t="s">
-        <v>12</v>
-      </c>
-      <c r="F4" t="n">
-        <v>172</v>
-      </c>
-      <c r="J4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F4" t="s">
+        <v>11</v>
+      </c>
+      <c r="H4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
+      <c r="A5" t="s">
         <v>17</v>
       </c>
-      <c r="K4" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11">
-      <c r="A5" t="s">
-        <v>19</v>
-      </c>
-      <c r="B5" s="1"/>
+      <c r="B5" s="1" t="s">
+        <v>9</v>
+      </c>
       <c r="C5" t="n">
         <v>2</v>
       </c>
@@ -763,44 +720,42 @@
         <v>3</v>
       </c>
       <c r="E5" t="s">
-        <v>12</v>
-      </c>
-      <c r="F5" t="n">
-        <v>172</v>
+        <v>10</v>
+      </c>
+      <c r="F5" t="s">
+        <v>11</v>
       </c>
       <c r="G5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
+      <c r="A6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" t="n">
+        <v>1</v>
+      </c>
+      <c r="D6" t="n">
+        <v>1</v>
+      </c>
+      <c r="E6" t="s">
         <v>20</v>
       </c>
-      <c r="K5" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11">
-      <c r="A6" t="s">
+      <c r="F6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
+      <c r="A7" t="s">
         <v>21</v>
       </c>
-      <c r="B6" s="1"/>
-      <c r="C6" t="n">
-        <v>1</v>
-      </c>
-      <c r="D6" t="n">
-        <v>1</v>
-      </c>
-      <c r="E6" t="s">
-        <v>22</v>
-      </c>
-      <c r="F6" t="n">
-        <v>172</v>
-      </c>
-      <c r="K6" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11">
-      <c r="A7" t="s">
-        <v>23</v>
-      </c>
-      <c r="B7" s="1"/>
+      <c r="B7" s="1" t="s">
+        <v>9</v>
+      </c>
       <c r="C7" t="n">
         <v>3</v>
       </c>
@@ -808,43 +763,39 @@
         <v>3</v>
       </c>
       <c r="E7" t="s">
-        <v>12</v>
-      </c>
-      <c r="F7" t="n">
-        <v>172</v>
-      </c>
-      <c r="K7" t="s">
+        <v>10</v>
+      </c>
+      <c r="F7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9">
+      <c r="A8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" t="n">
+        <v>1</v>
+      </c>
+      <c r="D8" t="n">
+        <v>1</v>
+      </c>
+      <c r="E8" t="s">
+        <v>20</v>
+      </c>
+      <c r="F8" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9">
+      <c r="A9" t="s">
+        <v>23</v>
+      </c>
+      <c r="B9" s="1" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="8" spans="1:11">
-      <c r="A8" t="s">
-        <v>24</v>
-      </c>
-      <c r="B8" s="1"/>
-      <c r="C8" t="n">
-        <v>1</v>
-      </c>
-      <c r="D8" t="n">
-        <v>1</v>
-      </c>
-      <c r="E8" t="s">
-        <v>22</v>
-      </c>
-      <c r="F8" t="n">
-        <v>172</v>
-      </c>
-      <c r="K8" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11">
-      <c r="A9" t="s">
-        <v>25</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>16</v>
-      </c>
       <c r="C9" t="n">
         <v>1</v>
       </c>
@@ -852,51 +803,45 @@
         <v>1</v>
       </c>
       <c r="E9" t="s">
-        <v>22</v>
-      </c>
-      <c r="F9" t="n">
-        <v>172</v>
-      </c>
-      <c r="J9" t="s">
-        <v>17</v>
-      </c>
-      <c r="K9" t="s">
-        <v>14</v>
+        <v>20</v>
+      </c>
+      <c r="F9" t="s">
+        <v>11</v>
+      </c>
+      <c r="H9" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="35" spans="1:1">
       <c r="A35" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="36" spans="1:1">
       <c r="A36" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
     </row>
     <row r="37" spans="1:1">
       <c r="A37" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="38" spans="1:1">
       <c r="A38" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>
-  <dataValidations count="2">
+  <dataValidations count="1">
     <dataValidation sqref="E2:E9" type="list" operator="between" errorStyle="stop" allowBlank="1" showInputMessage="1" showErrorMessage="1" view="0">
       <formula1>$A$37:$A$38</formula1>
-    </dataValidation>
-    <dataValidation sqref="K2:K9" type="list" operator="between" errorStyle="stop" allowBlank="1" showInputMessage="1" showErrorMessage="1" view="0">
-      <formula1>$A$35:$A$36</formula1>
     </dataValidation>
   </dataValidations>
   <printOptions>
     <extLst>
       <ext uri="smNativeData">
-        <pm:pageFlags xmlns:pm="smNativeData" id="1618575011" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
+        <pm:pageFlags xmlns:pm="smNativeData" id="1619371127" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
       </ext>
     </extLst>
   </printOptions>
@@ -905,8 +850,8 @@
   <headerFooter>
     <extLst>
       <ext uri="smNativeData">
-        <pm:header xmlns:pm="smNativeData" id="1618575011" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
-        <pm:footer xmlns:pm="smNativeData" id="1618575011" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
+        <pm:header xmlns:pm="smNativeData" id="1619371127" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
+        <pm:footer xmlns:pm="smNativeData" id="1619371127" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
       </ext>
     </extLst>
   </headerFooter>
@@ -915,7 +860,7 @@
   </tableParts>
   <extLst>
     <ext uri="smNativeData">
-      <pm:sheetPrefs xmlns:pm="smNativeData" day="1618575011" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
+      <pm:sheetPrefs xmlns:pm="smNativeData" day="1619371127" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
         <pm:shade id="0" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
         <pm:shade id="1" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
       </pm:sheetPrefs>
@@ -926,28 +871,31 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:N32"/>
+  <dimension ref="A1:L32"/>
   <sheetViews>
-    <sheetView view="normal" workbookViewId="0">
-      <selection activeCell="N6" sqref="N1:N6"/>
+    <sheetView tabSelected="1" view="normal" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3:F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.660714" defaultRowHeight="15.40"/>
   <cols>
     <col min="1" max="1" width="24.000000" customWidth="1"/>
-    <col min="2" max="2" width="16.553571" customWidth="1"/>
+    <col min="2" max="2" width="22.062500" customWidth="1"/>
     <col min="3" max="3" width="15.214286" customWidth="1"/>
-    <col min="4" max="4" width="15.553571" customWidth="1"/>
+    <col min="4" max="4" width="19.625000" customWidth="1"/>
+    <col min="5" max="5" width="18.794643" customWidth="1"/>
+    <col min="6" max="6" width="14.857143" customWidth="1"/>
     <col min="7" max="7" width="16.776786" customWidth="1"/>
-    <col min="14" max="14" width="17.660714" customWidth="1"/>
+    <col min="8" max="8" width="17.616071" customWidth="1"/>
+    <col min="11" max="11" width="17.660714" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:9">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>27</v>
+        <v>1</v>
       </c>
       <c r="C1" t="s">
         <v>2</v>
@@ -967,56 +915,38 @@
       <c r="H1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" t="s">
+    </row>
+    <row r="2" spans="1:12">
+      <c r="A2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2" t="n">
+        <v>1</v>
+      </c>
+      <c r="D2" t="n">
+        <v>1</v>
+      </c>
+      <c r="E2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="2" spans="1:14">
-      <c r="A2" t="s">
+      <c r="F2" t="s">
         <v>28</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="G2" t="s">
         <v>29</v>
       </c>
-      <c r="C2" t="n">
-        <v>1</v>
-      </c>
-      <c r="D2" t="n">
-        <v>1</v>
-      </c>
-      <c r="E2" t="s">
-        <v>12</v>
-      </c>
-      <c r="F2" t="n">
-        <v>157</v>
-      </c>
-      <c r="G2" t="s">
+      <c r="H2" s="3"/>
+      <c r="K2" s="3"/>
+    </row>
+    <row r="3" spans="1:9">
+      <c r="A3" t="s">
         <v>30</v>
       </c>
-      <c r="H2" s="3" t="n">
-        <v>44346</v>
-      </c>
-      <c r="I2" s="3" t="n">
-        <v>44367</v>
-      </c>
-      <c r="J2" s="3"/>
-      <c r="K2" t="s">
-        <v>14</v>
-      </c>
-      <c r="N2" s="3"/>
-    </row>
-    <row r="3" spans="1:11">
-      <c r="A3" t="s">
-        <v>31</v>
-      </c>
       <c r="B3" s="1" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="C3" t="n">
         <v>2</v>
@@ -1025,24 +955,21 @@
         <v>3</v>
       </c>
       <c r="E3" t="s">
-        <v>12</v>
-      </c>
-      <c r="F3" t="n">
-        <v>157</v>
+        <v>10</v>
+      </c>
+      <c r="F3" t="s">
+        <v>28</v>
       </c>
       <c r="G3" t="s">
-        <v>33</v>
-      </c>
-      <c r="K3" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
       <c r="A4" t="s">
-        <v>34</v>
-      </c>
-      <c r="B4" t="s">
-        <v>35</v>
+        <v>32</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>27</v>
       </c>
       <c r="C4" t="n">
         <v>2</v>
@@ -1051,24 +978,21 @@
         <v>4</v>
       </c>
       <c r="E4" t="s">
-        <v>12</v>
-      </c>
-      <c r="F4" t="n">
-        <v>157</v>
+        <v>10</v>
+      </c>
+      <c r="F4" t="s">
+        <v>28</v>
       </c>
       <c r="G4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
+      <c r="A5" t="s">
         <v>33</v>
       </c>
-      <c r="K4" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11">
-      <c r="A5" t="s">
-        <v>36</v>
-      </c>
-      <c r="B5" t="s">
-        <v>37</v>
+      <c r="B5" s="1" t="s">
+        <v>27</v>
       </c>
       <c r="C5" t="n">
         <v>1</v>
@@ -1077,24 +1001,21 @@
         <v>1</v>
       </c>
       <c r="E5" t="s">
-        <v>22</v>
-      </c>
-      <c r="F5" t="n">
-        <v>157</v>
+        <v>20</v>
+      </c>
+      <c r="F5" t="s">
+        <v>28</v>
       </c>
       <c r="G5" t="s">
-        <v>30</v>
-      </c>
-      <c r="K5" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
       <c r="A6" t="s">
-        <v>38</v>
-      </c>
-      <c r="B6" t="s">
-        <v>37</v>
+        <v>34</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>27</v>
       </c>
       <c r="C6" t="n">
         <v>1</v>
@@ -1103,21 +1024,18 @@
         <v>4</v>
       </c>
       <c r="E6" t="s">
-        <v>12</v>
-      </c>
-      <c r="F6" t="n">
-        <v>157</v>
-      </c>
-      <c r="K6" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11">
+        <v>10</v>
+      </c>
+      <c r="F6" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
       <c r="A7" t="s">
-        <v>39</v>
-      </c>
-      <c r="B7" t="s">
-        <v>40</v>
+        <v>35</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>27</v>
       </c>
       <c r="C7" t="n">
         <v>1</v>
@@ -1126,21 +1044,18 @@
         <v>2</v>
       </c>
       <c r="E7" t="s">
-        <v>22</v>
-      </c>
-      <c r="F7" t="n">
-        <v>157</v>
-      </c>
-      <c r="K7" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11">
+        <v>20</v>
+      </c>
+      <c r="F7" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9">
       <c r="A8" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="C8" t="n">
         <v>1</v>
@@ -1149,48 +1064,42 @@
         <v>3</v>
       </c>
       <c r="E8" t="s">
-        <v>22</v>
-      </c>
-      <c r="F8" t="n">
-        <v>157</v>
-      </c>
-      <c r="K8" t="s">
-        <v>26</v>
+        <v>20</v>
+      </c>
+      <c r="F8" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="29" spans="1:1">
       <c r="A29" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="30" spans="1:1">
       <c r="A30" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
     </row>
     <row r="31" spans="1:1">
       <c r="A31" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="32" spans="1:1">
       <c r="A32" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>
-  <dataValidations count="2">
+  <dataValidations count="1">
     <dataValidation sqref="E2:E8" type="list" operator="between" errorStyle="stop" allowBlank="1" showInputMessage="1" showErrorMessage="1" view="0">
       <formula1>$A$31:$A$32</formula1>
-    </dataValidation>
-    <dataValidation sqref="K2:K8" type="list" operator="between" errorStyle="stop" allowBlank="1" showInputMessage="1" showErrorMessage="1" view="0">
-      <formula1>$A$29:$A$30</formula1>
     </dataValidation>
   </dataValidations>
   <printOptions>
     <extLst>
       <ext uri="smNativeData">
-        <pm:pageFlags xmlns:pm="smNativeData" id="1618575011" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
+        <pm:pageFlags xmlns:pm="smNativeData" id="1619371127" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
       </ext>
     </extLst>
   </printOptions>
@@ -1199,8 +1108,8 @@
   <headerFooter>
     <extLst>
       <ext uri="smNativeData">
-        <pm:header xmlns:pm="smNativeData" id="1618575011" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
-        <pm:footer xmlns:pm="smNativeData" id="1618575011" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
+        <pm:header xmlns:pm="smNativeData" id="1619371127" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
+        <pm:footer xmlns:pm="smNativeData" id="1619371127" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
       </ext>
     </extLst>
   </headerFooter>
@@ -1209,7 +1118,7 @@
   </tableParts>
   <extLst>
     <ext uri="smNativeData">
-      <pm:sheetPrefs xmlns:pm="smNativeData" day="1618575011" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
+      <pm:sheetPrefs xmlns:pm="smNativeData" day="1619371127" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
         <pm:shade id="0" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
         <pm:shade id="1" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
       </pm:sheetPrefs>

</xml_diff>

<commit_message>
Ca marche pas, mais mieux
</commit_message>
<xml_diff>
--- a/examparams.xlsx
+++ b/examparams.xlsx
@@ -5,7 +5,7 @@
   <fileSharing readOnlyRecommended="0" userName="sputnik"/>
   <workbookPr/>
   <bookViews>
-    <workbookView activeTab="1" xWindow="240" yWindow="60" windowWidth="23246" windowHeight="12578" tabRatio="500"/>
+    <workbookView activeTab="0" xWindow="240" yWindow="60" windowWidth="23246" windowHeight="12578" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="172 POL" sheetId="1" r:id="rId4"/>
@@ -14,10 +14,10 @@
   <calcPr/>
   <extLst>
     <ext uri="smNativeData">
-      <pm:revision xmlns:pm="smNativeData" day="1619371127" val="982" rev="124" rev64="64" revOS="3" revMin="124" revMax="0"/>
-      <pm:docPrefs xmlns:pm="smNativeData" id="1619371127" fixedDigits="0" showNotice="1" showFrameBounds="1" autoChart="1" recalcOnPrint="1" recalcOnCopy="1" finalRounding="1" compatTextArt="1" tab="567" useDefinedPrintRange="1" printArea="currentSheet"/>
-      <pm:compatibility xmlns:pm="smNativeData" id="1619371127" overlapCells="1"/>
-      <pm:defCurrency xmlns:pm="smNativeData" id="1619371127"/>
+      <pm:revision xmlns:pm="smNativeData" day="1619802990" val="982" rev="124" rev64="64" revOS="3" revMin="124" revMax="0"/>
+      <pm:docPrefs xmlns:pm="smNativeData" id="1619802990" fixedDigits="0" showNotice="1" showFrameBounds="1" autoChart="1" recalcOnPrint="1" recalcOnCopy="1" finalRounding="1" compatTextArt="1" tab="567" useDefinedPrintRange="1" printArea="currentSheet"/>
+      <pm:compatibility xmlns:pm="smNativeData" id="1619802990" overlapCells="1"/>
+      <pm:defCurrency xmlns:pm="smNativeData" id="1619802990"/>
     </ext>
   </extLst>
 </workbook>
@@ -161,7 +161,7 @@
       <sz val="11"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1619371127" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1619802990" ulstyle="none" kern="1">
             <pm:latin face="Calibri" sz="220" lang="default"/>
             <pm:cs face="Basic Roman" sz="220" lang="default"/>
             <pm:ea face="Basic Roman" sz="220" lang="default"/>
@@ -176,7 +176,7 @@
       <sz val="10"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1619371127" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1619802990" ulstyle="none" kern="1">
             <pm:latin face="Basic Sans" sz="200" lang="default"/>
             <pm:cs face="Basic Roman" sz="200" lang="default"/>
             <pm:ea face="Basic Roman" sz="200" lang="default"/>
@@ -198,7 +198,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1619371127" type="1" fgLvl="100" fgClr="00000000" bgLvl="100" bgClr="00000000"/>
+            <pm:shade xmlns:pm="smNativeData" id="1619802990" type="1" fgLvl="100" fgClr="00000000" bgLvl="100" bgClr="00000000"/>
           </ext>
         </extLst>
       </patternFill>
@@ -209,7 +209,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1619371127" type="1" fgLvl="100" fgClr="00FFFFFF" bgLvl="100" bgClr="00000000"/>
+            <pm:shade xmlns:pm="smNativeData" id="1619802990" type="1" fgLvl="100" fgClr="00FFFFFF" bgLvl="100" bgClr="00000000"/>
           </ext>
         </extLst>
       </patternFill>
@@ -231,7 +231,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1619371127"/>
+          <pm:border xmlns:pm="smNativeData" id="1619802990"/>
         </ext>
       </extLst>
     </border>
@@ -250,7 +250,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1619371127"/>
+          <pm:border xmlns:pm="smNativeData" id="1619802990"/>
         </ext>
       </extLst>
     </border>
@@ -269,7 +269,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1619371127"/>
+          <pm:border xmlns:pm="smNativeData" id="1619802990"/>
         </ext>
       </extLst>
     </border>
@@ -291,10 +291,10 @@
   <tableStyles count="0"/>
   <extLst>
     <ext uri="smNativeData">
-      <pm:charStyles xmlns:pm="smNativeData" id="1619371127" count="1">
+      <pm:charStyles xmlns:pm="smNativeData" id="1619802990" count="1">
         <pm:charStyle name="Normal" fontId="0" Id="1"/>
       </pm:charStyles>
-      <pm:colors xmlns:pm="smNativeData" id="1619371127" count="2">
+      <pm:colors xmlns:pm="smNativeData" id="1619802990" count="2">
         <pm:color name="Color 24" rgb="E26B0A"/>
         <pm:color name="Color 25" rgb="C2D69A"/>
       </pm:colors>
@@ -593,10 +593,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I38"/>
+  <dimension ref="A1:H38"/>
   <sheetViews>
-    <sheetView view="normal" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3:F9"/>
+    <sheetView tabSelected="1" view="normal" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.660714" defaultRowHeight="15.40"/>
@@ -610,7 +610,7 @@
     <col min="8" max="8" width="14.330357" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:8">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -636,7 +636,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:8">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -660,7 +660,7 @@
       </c>
       <c r="H2" s="3"/>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:8">
       <c r="A3" t="s">
         <v>13</v>
       </c>
@@ -668,7 +668,7 @@
         <v>14</v>
       </c>
       <c r="C3" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D3" t="n">
         <v>1</v>
@@ -683,7 +683,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:8">
       <c r="A4" t="s">
         <v>16</v>
       </c>
@@ -691,7 +691,7 @@
         <v>14</v>
       </c>
       <c r="C4" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D4" t="n">
         <v>1</v>
@@ -706,7 +706,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:9">
+    <row r="5" spans="1:7">
       <c r="A5" t="s">
         <v>17</v>
       </c>
@@ -729,7 +729,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:9">
+    <row r="6" spans="1:6">
       <c r="A6" t="s">
         <v>19</v>
       </c>
@@ -749,7 +749,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:9">
+    <row r="7" spans="1:6">
       <c r="A7" t="s">
         <v>21</v>
       </c>
@@ -769,7 +769,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:9">
+    <row r="8" spans="1:6">
       <c r="A8" t="s">
         <v>22</v>
       </c>
@@ -789,7 +789,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:9">
+    <row r="9" spans="1:8">
       <c r="A9" t="s">
         <v>23</v>
       </c>
@@ -841,7 +841,7 @@
   <printOptions>
     <extLst>
       <ext uri="smNativeData">
-        <pm:pageFlags xmlns:pm="smNativeData" id="1619371127" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
+        <pm:pageFlags xmlns:pm="smNativeData" id="1619802990" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
       </ext>
     </extLst>
   </printOptions>
@@ -850,8 +850,8 @@
   <headerFooter>
     <extLst>
       <ext uri="smNativeData">
-        <pm:header xmlns:pm="smNativeData" id="1619371127" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
-        <pm:footer xmlns:pm="smNativeData" id="1619371127" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
+        <pm:header xmlns:pm="smNativeData" id="1619802990" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
+        <pm:footer xmlns:pm="smNativeData" id="1619802990" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
       </ext>
     </extLst>
   </headerFooter>
@@ -860,7 +860,7 @@
   </tableParts>
   <extLst>
     <ext uri="smNativeData">
-      <pm:sheetPrefs xmlns:pm="smNativeData" day="1619371127" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
+      <pm:sheetPrefs xmlns:pm="smNativeData" day="1619802990" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
         <pm:shade id="0" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
         <pm:shade id="1" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
       </pm:sheetPrefs>
@@ -871,9 +871,9 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L32"/>
+  <dimension ref="A1:K32"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="normal" workbookViewId="0">
+    <sheetView view="normal" workbookViewId="0">
       <selection activeCell="F3" sqref="F3:F8"/>
     </sheetView>
   </sheetViews>
@@ -890,7 +890,7 @@
     <col min="11" max="11" width="17.660714" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:8">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -916,7 +916,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:12">
+    <row r="2" spans="1:11">
       <c r="A2" t="s">
         <v>26</v>
       </c>
@@ -941,7 +941,7 @@
       <c r="H2" s="3"/>
       <c r="K2" s="3"/>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:7">
       <c r="A3" t="s">
         <v>30</v>
       </c>
@@ -964,7 +964,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:7">
       <c r="A4" t="s">
         <v>32</v>
       </c>
@@ -987,7 +987,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="5" spans="1:9">
+    <row r="5" spans="1:7">
       <c r="A5" t="s">
         <v>33</v>
       </c>
@@ -1010,7 +1010,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="1:9">
+    <row r="6" spans="1:6">
       <c r="A6" t="s">
         <v>34</v>
       </c>
@@ -1030,7 +1030,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="7" spans="1:9">
+    <row r="7" spans="1:6">
       <c r="A7" t="s">
         <v>35</v>
       </c>
@@ -1050,7 +1050,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="8" spans="1:9">
+    <row r="8" spans="1:6">
       <c r="A8" t="s">
         <v>36</v>
       </c>
@@ -1099,7 +1099,7 @@
   <printOptions>
     <extLst>
       <ext uri="smNativeData">
-        <pm:pageFlags xmlns:pm="smNativeData" id="1619371127" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
+        <pm:pageFlags xmlns:pm="smNativeData" id="1619802990" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
       </ext>
     </extLst>
   </printOptions>
@@ -1108,8 +1108,8 @@
   <headerFooter>
     <extLst>
       <ext uri="smNativeData">
-        <pm:header xmlns:pm="smNativeData" id="1619371127" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
-        <pm:footer xmlns:pm="smNativeData" id="1619371127" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
+        <pm:header xmlns:pm="smNativeData" id="1619802990" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
+        <pm:footer xmlns:pm="smNativeData" id="1619802990" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
       </ext>
     </extLst>
   </headerFooter>
@@ -1118,7 +1118,7 @@
   </tableParts>
   <extLst>
     <ext uri="smNativeData">
-      <pm:sheetPrefs xmlns:pm="smNativeData" day="1619371127" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
+      <pm:sheetPrefs xmlns:pm="smNativeData" day="1619802990" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
         <pm:shade id="0" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
         <pm:shade id="1" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
       </pm:sheetPrefs>

</xml_diff>

<commit_message>
fix petit bug d'import
</commit_message>
<xml_diff>
--- a/examparams.xlsx
+++ b/examparams.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23530"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\laris\OneDrive\Documents\ERM\1Ma2Sem\DS425 - (6) AI Decision support\PROJECT1\ExamTimetable\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Romain\Documents\ERM\1Ma\DS425_E\Practicals_work\Projects\ExamTimetable\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45759B41-5A4C-4B81-B5BB-AB530235CF7B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4BDF535-4597-465E-84A7-8BA6A3B482AE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5292" yWindow="2616" windowWidth="17280" windowHeight="8964" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="172 POL" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="44">
   <si>
     <t>Name</t>
   </si>
@@ -111,12 +111,6 @@
   </si>
   <si>
     <t>SE422_written</t>
-  </si>
-  <si>
-    <t>yes</t>
-  </si>
-  <si>
-    <t>no</t>
   </si>
   <si>
     <t>157SSMW</t>
@@ -184,8 +178,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="172" formatCode="h:mm"/>
-    <numFmt numFmtId="173" formatCode="m/d/yyyy"/>
+    <numFmt numFmtId="164" formatCode="h:mm"/>
+    <numFmt numFmtId="165" formatCode="m/d/yyyy"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -217,11 +211,11 @@
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="172" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
       <protection hidden="1"/>
     </xf>
-    <xf numFmtId="173" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="1"/>
@@ -557,8 +551,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -603,7 +597,7 @@
         <v>8</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -673,7 +667,7 @@
         <v>17</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C5">
         <v>2</v>
@@ -696,7 +690,7 @@
         <v>19</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C6">
         <v>1</v>
@@ -736,7 +730,7 @@
         <v>22</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C8">
         <v>1</v>
@@ -774,25 +768,11 @@
         <v>15</v>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A35" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A36" t="s">
-        <v>25</v>
-      </c>
-    </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A37" s="2" t="s">
-        <v>10</v>
-      </c>
+      <c r="A37" s="2"/>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A38" s="2" t="s">
-        <v>20</v>
-      </c>
+      <c r="A38" s="2"/>
     </row>
   </sheetData>
   <dataValidations count="1">
@@ -820,7 +800,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25B85FAA-7521-4D32-80E7-BEE49E473068}">
   <dimension ref="A1:H3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
@@ -854,10 +834,10 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -869,19 +849,19 @@
         <v>10</v>
       </c>
       <c r="F2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="G2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="H2" s="3"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C3">
         <v>1</v>
@@ -893,10 +873,10 @@
         <v>10</v>
       </c>
       <c r="F3" t="s">
+        <v>41</v>
+      </c>
+      <c r="G3" t="s">
         <v>43</v>
-      </c>
-      <c r="G3" t="s">
-        <v>45</v>
       </c>
     </row>
   </sheetData>
@@ -916,8 +896,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:K30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="A27" sqref="A27:A30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -961,10 +941,10 @@
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -976,20 +956,20 @@
         <v>10</v>
       </c>
       <c r="F2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="G2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="H2" s="3"/>
       <c r="K2" s="3"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C3">
         <v>2</v>
@@ -1001,18 +981,18 @@
         <v>10</v>
       </c>
       <c r="F3" t="s">
+        <v>24</v>
+      </c>
+      <c r="G3" t="s">
         <v>26</v>
-      </c>
-      <c r="G3" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C4">
         <v>2</v>
@@ -1024,18 +1004,18 @@
         <v>10</v>
       </c>
       <c r="F4" t="s">
+        <v>24</v>
+      </c>
+      <c r="G4" t="s">
         <v>26</v>
-      </c>
-      <c r="G4" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C5">
         <v>1</v>
@@ -1047,18 +1027,18 @@
         <v>20</v>
       </c>
       <c r="F5" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="G5" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C6">
         <v>1</v>
@@ -1070,28 +1050,14 @@
         <v>10</v>
       </c>
       <c r="F6" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A27" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A28" t="s">
-        <v>25</v>
-      </c>
-    </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A29" s="2" t="s">
-        <v>10</v>
-      </c>
+      <c r="A29" s="2"/>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A30" s="2" t="s">
-        <v>20</v>
-      </c>
+      <c r="A30" s="2"/>
     </row>
   </sheetData>
   <dataValidations count="1">

</xml_diff>